<commit_message>
add 5 year limit since migration
</commit_message>
<xml_diff>
--- a/tables/consent/forms/consent/consent.xlsx
+++ b/tables/consent/forms/consent/consent.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="225">
   <si>
     <t xml:space="preserve">setting_name</t>
   </si>
@@ -2246,6 +2246,98 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">less_than_5 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;span style="font-weight:bold"&gt;Do you confirm you have been in Thailand for less than 5 years?&lt;/div&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;span style="font-weight:bold"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ခင်ဗျားကထိုင်းနိုင်ငံကိုရောက်လာတာ ၅ နှစ်ထက်ပိုမကြာကြောင်း အတည်ပြုပါသလား။</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;/div&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">more_than_5 years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unfortunately, we are only interviewing migrants that arrived in last 5 years because otherwise it might be difficult for you to remember about your migration process. I am sorry we cannot interview you today, but thank you for your interest and time.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">စိတ်မကောင်းပါဘူး။ ကျွန်တော်</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ကျွန်မက လွန်ခဲ့​သော ၅ နှစ် မှရောက်လာသော ရွေ့ပြောင်းအလုပ်သမားကိုသာ မေးမြန်ပါသည်။ ဘာ​ကြောင့်လဲဆိုတော့ ခင်ဗျားက ခင်ဗျားရဲ့ ဘယ်လိုရွေ့ပြောင်းခဲ့လဲဆိုတဲ့အကြောင်းကိုကောင်းကောင်းမှတ်မိမှာမဟုတ်လို့ဖြစ်တယ်</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">စိတ်မကောင်းပါဘူး။ ခင်ဗျားကိုဒီနေ့မေးမြန်းလို့မရပါဘူး။ ခင်ဗျားရဲ့ အချိန်ပေးမှုနှင့် စိတ်၀င်စားမှုအတွက်အရမ်းကိုကျေးဇူးတင်ပါတယ်။</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">branch_label</t>
   </si>
   <si>
@@ -2321,10 +2413,25 @@
     <t xml:space="preserve">end screen</t>
   </si>
   <si>
+    <t xml:space="preserve">adult</t>
+  </si>
+  <si>
     <t xml:space="preserve">if</t>
   </si>
   <si>
     <t xml:space="preserve">calculates.is_adult()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lessThanFiveYears</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculates.less_than_five_years()</t>
   </si>
   <si>
     <t xml:space="preserve">text</t>
@@ -2391,9 +2498,6 @@
   </si>
   <si>
     <t xml:space="preserve">Than Cho</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luke DeMarest</t>
   </si>
   <si>
     <t xml:space="preserve">yes</t>
@@ -2492,6 +2596,33 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">facebook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facebook</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ဖေ့စ်ဘို့ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(Facebook)</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">other</t>
   </si>
   <si>
@@ -2549,6 +2680,72 @@
     <t xml:space="preserve">မမှာ ဒီနေ့ အချိန်မအားလို့ပါ</t>
   </si>
   <si>
+    <t xml:space="preserve">Yes, I have been in Thailand for less than 5 years</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ဟုတ်ကဲ့ ကျွန်တော်</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ကျွန်မဟာ ဒီထိုင်းနိုင်ငံကို ရောက်တာ ၅နှစ်ထက်မပိုပါဘူး</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">No, I have been in Thailand for more than 5 years</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">မဟုတ်ပါ။ ကျွန်တော်</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ကျွန်မဟာ ဒီထိုင်းနိုင်ငံကို ရောက်တာ ၅နှစ်ထက် ပိုကျော်သွားပါပြီ။</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">comment</t>
   </si>
   <si>
@@ -2580,6 +2777,12 @@
   </si>
   <si>
     <t xml:space="preserve">selected(data("reasonRefusal"), "other")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">less_than_five_years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(data("lessThanFiveYears"), "yes")</t>
   </si>
 </sst>
 </file>
@@ -2736,10 +2939,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2749,6 +2948,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2777,10 +2980,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0959595959596"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5606060606061"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.1717171717172"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="19.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8282828282828"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2929292929293"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="17.6414141414141"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="19.2424242424242"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.41919191919192"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="18.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2889,17 +3094,17 @@
   </sheetPr>
   <dimension ref="1:62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="29.2626262626263"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="45.1666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="45.4343434343434"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="116.121212121212"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="5" width="4.14141414141414"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="28.5959595959596"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="44.0959595959596"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="44.3636363636364"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="113.717171717172"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="5" width="4.01010101010101"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38026,10 +38231,17 @@
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
+      <c r="B41" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6"/>
@@ -38046,10 +38258,17 @@
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
+      <c r="B45" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6"/>
@@ -38152,29 +38371,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:58"/>
+  <dimension ref="1:67"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I31" activeCellId="0" sqref="I31"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.68686868686869"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.0252525252525"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3585858585859"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.3434343434343"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.4646464646465"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.7070707070707"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.0454545454545"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.2474747474747"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.2323232323232"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.88888888888889"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.8282828282828"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.6414141414141"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.2424242424242"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="20.3131313131313"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.3737373737374"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6262626262626"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0909090909091"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.540404040404"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.7929292929293"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3080808080808"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.510101010101"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.8484848484848"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.9646464646465"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.62121212121212"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.5606060606061"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.1060606060606"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.8434343434343"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="19.7777777777778"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.9747474747475"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.41919191919192"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -38182,67 +38405,67 @@
         <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="V1" s="2" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="AMJ1" s="7"/>
     </row>
@@ -38268,7 +38491,7 @@
     </row>
     <row r="3" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C3" s="7" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -38284,7 +38507,7 @@
         <v>20</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="6"/>
@@ -38297,7 +38520,7 @@
         <v>23</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="6"/>
@@ -38309,13 +38532,13 @@
         <v>26</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>1</v>
@@ -38326,7 +38549,7 @@
         <v>29</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -38336,7 +38559,7 @@
         <v>32</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="8"/>
@@ -38346,7 +38569,7 @@
         <v>35</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
@@ -38356,7 +38579,7 @@
         <v>38</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>38</v>
@@ -38370,407 +38593,504 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="7" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="E11" s="8"/>
     </row>
     <row r="12" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="E12" s="14"/>
+      <c r="A12" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="7" t="s">
-        <v>135</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="D13" s="7"/>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="7"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E15" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>143</v>
-      </c>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8"/>
     </row>
-    <row r="16" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E16" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="I16" s="0" t="n">
-        <v>1</v>
-      </c>
+    <row r="16" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="E16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+      <c r="C17" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="E17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="D18" s="7"/>
+      <c r="C18" s="7"/>
       <c r="E18" s="8"/>
+      <c r="F18" s="7"/>
     </row>
-    <row r="19" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="E19" s="14"/>
+    <row r="19" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="8"/>
+    <row r="20" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E20" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="8"/>
-      <c r="F21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="7"/>
+      <c r="C22" s="7" t="s">
+        <v>145</v>
+      </c>
       <c r="D22" s="7"/>
       <c r="E22" s="8"/>
-      <c r="F22" s="7"/>
     </row>
-    <row r="23" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E23" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>47</v>
-      </c>
+    <row r="23" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="E23" s="13"/>
     </row>
-    <row r="24" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E24" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>147</v>
-      </c>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="8"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>148</v>
-      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
       <c r="E25" s="8"/>
       <c r="F25" s="7"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
     </row>
-    <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E26" s="9" t="s">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E27" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E28" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+    </row>
+    <row r="30" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F26" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="H26" s="8"/>
+      <c r="F30" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="H30" s="8"/>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-    </row>
-    <row r="28" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E28" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E29" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E30" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E31" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="I31" s="0" t="n">
-        <v>1</v>
-      </c>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E31" s="8"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
     </row>
     <row r="32" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E32" s="9" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="I32" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="P32" s="7"/>
+        <v>142</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E33" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E34" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="I35" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="I36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P36" s="7"/>
+    </row>
+    <row r="37" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E37" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="F37" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="G33" s="7" t="s">
+      <c r="G37" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="I33" s="0" t="n">
+      <c r="I37" s="0" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="7"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="36" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="13" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="7" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
+      <c r="C39" s="7" t="s">
+        <v>145</v>
+      </c>
     </row>
-    <row r="40" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E40" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>136</v>
+    <row r="40" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>163</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E41" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>136</v>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="7" t="s">
+        <v>141</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E42" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="H42" s="7" t="s">
-        <v>153</v>
-      </c>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="E43" s="8"/>
+      <c r="C43" s="7"/>
+      <c r="E43" s="7"/>
       <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
     </row>
-    <row r="44" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E44" s="9" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F44" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="G44" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="H44" s="7"/>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="E45" s="8"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
+    <row r="45" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E45" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>142</v>
+      </c>
     </row>
-    <row r="46" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E46" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>136</v>
+        <v>143</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E47" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>136</v>
-      </c>
+      <c r="C47" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E47" s="8"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
     </row>
     <row r="48" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E48" s="9" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>156</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="H48" s="7"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="7" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="E49" s="8"/>
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
     </row>
-    <row r="50" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C50" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="E50" s="14"/>
+    <row r="50" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E50" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>142</v>
+      </c>
     </row>
-    <row r="51" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C51" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="E51" s="14"/>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E51" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>142</v>
+      </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E52" s="8"/>
+    <row r="52" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E52" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C53" s="7"/>
+      <c r="C53" s="7" t="s">
+        <v>145</v>
+      </c>
       <c r="E53" s="8"/>
       <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E54" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F54" s="7" t="s">
-        <v>136</v>
-      </c>
+    <row r="54" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="E54" s="13"/>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E55" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>136</v>
+    <row r="55" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>163</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E56" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G56" s="7" t="s">
-        <v>157</v>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C56" s="7" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C57" s="5" t="s">
-        <v>139</v>
+      <c r="E57" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>142</v>
       </c>
     </row>
-    <row r="58" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C58" s="13" t="s">
-        <v>150</v>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C58" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="59" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="60" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="E60" s="13"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C61" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E61" s="8"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C62" s="7"/>
+      <c r="E62" s="8"/>
+      <c r="F62" s="7"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E63" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E64" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E65" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G65" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C66" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="67" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -38789,19 +39109,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.4444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4494949494949"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.4040404040404"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.0353535353535"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1010101010101"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9090909090909"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.9141414141414"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.7323232323232"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.969696969697"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.41919191919192"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -38809,10 +39130,10 @@
         <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
@@ -38823,73 +39144,65 @@
     </row>
     <row r="3" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="9" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="9" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>161</v>
+        <v>172</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="9" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>162</v>
+        <v>173</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="9" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>164</v>
-      </c>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="8"/>
@@ -38908,13 +39221,13 @@
         <v>38</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -38922,13 +39235,13 @@
         <v>38</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -38939,30 +39252,30 @@
     </row>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="9" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="9" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38973,140 +39286,181 @@
     </row>
     <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="9" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="9" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="9" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="9" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="9" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="D20" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B21" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E21" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-    </row>
-    <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>188</v>
-      </c>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="9" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="9" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="9" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="D25" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E26" s="8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B30" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -39123,30 +39477,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:19"/>
+  <dimension ref="1:21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.2979797979798"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3030303030303"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.4141414141414"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6969696969697"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.2575757575758"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.8989898989899"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9040404040404"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.6161616161616"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.2979797979798"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.7222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.41919191919192"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>120</v>
+        <v>212</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>126</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
@@ -39157,15 +39512,15 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="5" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="7" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>38</v>
@@ -39173,31 +39528,31 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="7" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="7" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="7" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="7" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>47</v>
@@ -39213,26 +39568,26 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="7" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="7" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="7" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39241,10 +39596,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="5" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39252,31 +39607,39 @@
         <v>68</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="7" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="7" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="7" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>120</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -39295,40 +39658,41 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1868686868687"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.4848484848485"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.520202020202"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.5505050505051"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.41919191919192"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>199</v>
+        <v>216</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>200</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>201</v>
+        <v>218</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39336,15 +39700,23 @@
         <v>53</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>205</v>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>